<commit_message>
Domin Expiry checker Initial commit every thing working fine except the verication of captha
</commit_message>
<xml_diff>
--- a/Myntra.xlsx
+++ b/Myntra.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ESoft_Solutions\AutomationPractice\BDD_Framework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{139BCD42-A206-430E-B2B7-C7B014A25E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE86D7EA-569A-47BB-AC95-F769121D4622}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1820" yWindow="1820" windowWidth="19200" windowHeight="10010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestData" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="149">
   <si>
     <t>Shirts</t>
   </si>
@@ -34,9 +34,6 @@
     <t>Sheos</t>
   </si>
   <si>
-    <t>Walets</t>
-  </si>
-  <si>
     <t>Home decore</t>
   </si>
   <si>
@@ -74,13 +71,416 @@
   </si>
   <si>
     <t>Date and Time</t>
+  </si>
+  <si>
+    <t>Allen Solly</t>
+  </si>
+  <si>
+    <t>Men Leather Two Fold Wallet</t>
+  </si>
+  <si>
+    <t>₹1104</t>
+  </si>
+  <si>
+    <t>United Colors of Benetton</t>
+  </si>
+  <si>
+    <t>₹549</t>
+  </si>
+  <si>
+    <t>Lino Perros</t>
+  </si>
+  <si>
+    <t>Women Maroon Croc Textured Zip Around Wallet</t>
+  </si>
+  <si>
+    <t>₹523</t>
+  </si>
+  <si>
+    <t>French Connection</t>
+  </si>
+  <si>
+    <t>Women Textured Leather Zip Around Wallet</t>
+  </si>
+  <si>
+    <t>₹539</t>
+  </si>
+  <si>
+    <t>T-Shirts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Suits</t>
+  </si>
+  <si>
+    <t>Jackets</t>
+  </si>
+  <si>
+    <t>bath towels</t>
+  </si>
+  <si>
+    <t>wallet</t>
+  </si>
+  <si>
+    <t>woodland</t>
+  </si>
+  <si>
+    <t>Rust Brown Safari Cotton Zero Twist Bath towel</t>
+  </si>
+  <si>
+    <t>₹714</t>
+  </si>
+  <si>
+    <t>DDecor</t>
+  </si>
+  <si>
+    <t>Multicoloured Solid 500 GSM Cotton Bath Towel</t>
+  </si>
+  <si>
+    <t>₹749</t>
+  </si>
+  <si>
+    <t>Twamev</t>
+  </si>
+  <si>
+    <t>Embroidered Sherwani Set</t>
+  </si>
+  <si>
+    <t>MRP₹ 49999</t>
+  </si>
+  <si>
+    <t>Masaba</t>
+  </si>
+  <si>
+    <t>Floral Printed Strapless Top With Trouser &amp; Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 50000</t>
+  </si>
+  <si>
+    <t>Just Cavalli</t>
+  </si>
+  <si>
+    <t>Embellished Zip Around Wallet</t>
+  </si>
+  <si>
+    <t>MRP₹ 13999</t>
+  </si>
+  <si>
+    <t>Polo Ralph Lauren</t>
+  </si>
+  <si>
+    <t>MRP₹ 14500</t>
+  </si>
+  <si>
+    <t>HACKETT LONDON</t>
+  </si>
+  <si>
+    <t>Polo Collar Short Sleeves Cotton T-shirt</t>
+  </si>
+  <si>
+    <t>MRP₹ 18500</t>
+  </si>
+  <si>
+    <t>Polo Collar Cotton T-shirt</t>
+  </si>
+  <si>
+    <t>Antar-Agni</t>
+  </si>
+  <si>
+    <t>Mandarin Collar Self Design Samurai Jacket with Pyjama Pants</t>
+  </si>
+  <si>
+    <t>MRP₹ 78000</t>
+  </si>
+  <si>
+    <t>THE HANDMADE FLAIR</t>
+  </si>
+  <si>
+    <t>Blue &amp; Yellow Wooden Wall Painting</t>
+  </si>
+  <si>
+    <t>MRP₹ 129599</t>
+  </si>
+  <si>
+    <t>Grey &amp; Black Abstract Wooden Wall Paintings</t>
+  </si>
+  <si>
+    <t>MRP₹ 151199</t>
+  </si>
+  <si>
+    <t>Heelium</t>
+  </si>
+  <si>
+    <t>Set Of 12 Teal Blue Solid 600 GSM Super Soft Quick Absorbent Bamboo Bath Towels</t>
+  </si>
+  <si>
+    <t>₹9999</t>
+  </si>
+  <si>
+    <t>Lightweight Longline Haath-Phool Raja Koti Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 60000</t>
+  </si>
+  <si>
+    <t>Quilted Mock Collar Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 69500</t>
+  </si>
+  <si>
+    <t>Roadster</t>
+  </si>
+  <si>
+    <t>The Life Co. Pure Cotton Solid Denim Trucker Jacket</t>
+  </si>
+  <si>
+    <t>₹943</t>
+  </si>
+  <si>
+    <t>SASSAFRAS</t>
+  </si>
+  <si>
+    <t>Women White Self-Striped Corduroy Crop Tailored Jacket</t>
+  </si>
+  <si>
+    <t>₹1034</t>
+  </si>
+  <si>
+    <t>Yellow Irregular Mirror Wall Decor</t>
+  </si>
+  <si>
+    <t>MRP₹ 128349</t>
+  </si>
+  <si>
+    <t>1 Piece Wood Abstract Wall Art</t>
+  </si>
+  <si>
+    <t>₹123983</t>
+  </si>
+  <si>
+    <t>Set Of 12 Grey Solid 600 GSM Quick Absorbent Bamboo Bath Towels</t>
+  </si>
+  <si>
+    <t>Karl Lagerfeld</t>
+  </si>
+  <si>
+    <t>Spread Collar Embroidered Formal Cotton Shirt</t>
+  </si>
+  <si>
+    <t>MRP₹ 29500</t>
+  </si>
+  <si>
+    <t>Van Heusen</t>
+  </si>
+  <si>
+    <t>Slim-Fit Single-Breasted Four-Piece Suit</t>
+  </si>
+  <si>
+    <t>MRP₹ 27999</t>
+  </si>
+  <si>
+    <t>NEHHA NHATA</t>
+  </si>
+  <si>
+    <t>Floral Embroidered Thread Work Pure Silk Kurta &amp; Trousers With Dupatta</t>
+  </si>
+  <si>
+    <t>MRP₹ 52000</t>
+  </si>
+  <si>
+    <t>Single-Breasted Slim-Fit Blazer</t>
+  </si>
+  <si>
+    <t>₹56250</t>
+  </si>
+  <si>
+    <t>5-Piece Self Design Suits</t>
+  </si>
+  <si>
+    <t>MRP₹ 29999</t>
+  </si>
+  <si>
+    <t>Blackberrys</t>
+  </si>
+  <si>
+    <t>Men 3-Piece Slim-Fit Single-Breasted Woolen Formal Suit</t>
+  </si>
+  <si>
+    <t>MRP₹ 34995</t>
+  </si>
+  <si>
+    <t>Jack &amp; Jones</t>
+  </si>
+  <si>
+    <t>Leather Two Fold Wallet</t>
+  </si>
+  <si>
+    <t>MRP₹ 1499</t>
+  </si>
+  <si>
+    <t>MUSH</t>
+  </si>
+  <si>
+    <t>Blue 4 Pcs Bamboo Bath Towels</t>
+  </si>
+  <si>
+    <t>MRP₹ 14392</t>
+  </si>
+  <si>
+    <t>Men Charcoal Grey Textured Slim Fit Formal Suit</t>
+  </si>
+  <si>
+    <t>₹25495</t>
+  </si>
+  <si>
+    <t>Slim-Fit Single-Breasted Three-Piece Formal Suit</t>
+  </si>
+  <si>
+    <t>Nautica</t>
+  </si>
+  <si>
+    <t>Men Tan Brown Solid Perforated Sneakers</t>
+  </si>
+  <si>
+    <t>₹1439</t>
+  </si>
+  <si>
+    <t>HRX by Hrithik Roshan</t>
+  </si>
+  <si>
+    <t>Men White And Grey Memory Foam Non-Marking Running Shoes</t>
+  </si>
+  <si>
+    <t>₹959</t>
+  </si>
+  <si>
+    <t>Nike</t>
+  </si>
+  <si>
+    <t>Men G.T. Cut 3 ASW EP Basketball Shoes</t>
+  </si>
+  <si>
+    <t>MRP₹ 18395</t>
+  </si>
+  <si>
+    <t>Men Air Jordan 3 Retro Craft Sneakers</t>
+  </si>
+  <si>
+    <t>MRP₹ 19295</t>
+  </si>
+  <si>
+    <t>Anko</t>
+  </si>
+  <si>
+    <t>White 4 Pieces Cotton 670 GSM Bath Towel</t>
+  </si>
+  <si>
+    <t>MRP₹ 4396</t>
+  </si>
+  <si>
+    <t>Story@home</t>
+  </si>
+  <si>
+    <t>Set of 4 Beige Striped 450GSM Pure Cotton Bath Towels</t>
+  </si>
+  <si>
+    <t>MRP₹ 5196</t>
+  </si>
+  <si>
+    <t>Mock Collar Cotton Bomber Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 34500</t>
+  </si>
+  <si>
+    <t>Fred Perry</t>
+  </si>
+  <si>
+    <t>Mandarin Collar Hooded Longline Padded Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 42500</t>
+  </si>
+  <si>
+    <t>GANT</t>
+  </si>
+  <si>
+    <t>Embroidered Detail Stand Collar Varsity Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 99999</t>
+  </si>
+  <si>
+    <t>Leather Biker Jacket</t>
+  </si>
+  <si>
+    <t>MRP₹ 85000</t>
+  </si>
+  <si>
+    <t>Ethnic Motifs Embroidered Sequinned Shahi Tukda Tissue Saree</t>
+  </si>
+  <si>
+    <t>MRP₹ 63000</t>
+  </si>
+  <si>
+    <t>MOKSHA DESIGNS</t>
+  </si>
+  <si>
+    <t>Woven Design Zari Pure Silk Kanjeevaram Saree</t>
+  </si>
+  <si>
+    <t>₹67056</t>
+  </si>
+  <si>
+    <t>Anjaneya Sarees</t>
+  </si>
+  <si>
+    <t>Ethnic Motifs Zari Chanderi Saree</t>
+  </si>
+  <si>
+    <t>KALINI</t>
+  </si>
+  <si>
+    <t>Women Blue Sarees</t>
+  </si>
+  <si>
+    <t>₹499</t>
+  </si>
+  <si>
+    <t>Blue &amp; White Mystical Deer Framed Painting Wall Art</t>
+  </si>
+  <si>
+    <t>₹70847</t>
+  </si>
+  <si>
+    <t>Brown &amp; Gold-Toned Abstract Framed Painting Wall Art</t>
+  </si>
+  <si>
+    <t>₹98399</t>
+  </si>
+  <si>
+    <t>Striped Zari Banarasi Saree</t>
+  </si>
+  <si>
+    <t>₹1079</t>
+  </si>
+  <si>
+    <t>Checked Zari Silk Banarasi Saree</t>
+  </si>
+  <si>
+    <t>₹1109</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,16 +488,67 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <bgColor indexed="52"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="53"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="1"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -105,12 +556,231 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top style="medium"/>
+    </border>
+    <border>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
+    <border>
+      <left style="medium"/>
+      <right style="medium"/>
+      <top style="medium"/>
+      <bottom style="medium"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyBorder="true" applyFill="true">
+      <alignment wrapText="true" vertical="top" horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,48 +1061,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="39" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="4.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="39.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="5.81640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="4.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -442,54 +1140,648 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95572E08-B2A5-42D5-8863-DC8E08610FF4}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="38.453125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.7265625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="38.453125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
       <c r="D1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>13</v>
       </c>
-      <c r="C3" t="s">
-        <v>14</v>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>49</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B22" t="s">
+        <v>64</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>76</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>61</v>
+      </c>
+      <c r="B28" t="s">
+        <v>78</v>
+      </c>
+      <c r="C28" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" t="s">
+        <v>80</v>
+      </c>
+      <c r="C29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>92</v>
+      </c>
+      <c r="B34" t="s">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s" s="2">
+        <v>98</v>
+      </c>
+      <c r="B36" t="s" s="3">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="s" s="5">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s" s="6">
+        <v>99</v>
+      </c>
+      <c r="C37" t="s" s="7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="s" s="8">
+        <v>92</v>
+      </c>
+      <c r="B38" t="s" s="9">
+        <v>101</v>
+      </c>
+      <c r="C38" t="s" s="10">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="s" s="11">
+        <v>82</v>
+      </c>
+      <c r="B39" t="s" s="12">
+        <v>103</v>
+      </c>
+      <c r="C39" t="s" s="13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="s" s="14">
+        <v>104</v>
+      </c>
+      <c r="B40" t="s" s="15">
+        <v>105</v>
+      </c>
+      <c r="C40" t="s" s="16">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="s" s="17">
+        <v>107</v>
+      </c>
+      <c r="B41" t="s" s="18">
+        <v>108</v>
+      </c>
+      <c r="C41" t="s" s="19">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>110</v>
+      </c>
+      <c r="B42" t="s">
+        <v>111</v>
+      </c>
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>110</v>
+      </c>
+      <c r="B43" t="s">
+        <v>113</v>
+      </c>
+      <c r="C43" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>115</v>
+      </c>
+      <c r="B44" t="s">
+        <v>116</v>
+      </c>
+      <c r="C44" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45" t="s">
+        <v>119</v>
+      </c>
+      <c r="C45" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="s" s="32">
+        <v>49</v>
+      </c>
+      <c r="B46" t="s" s="33">
+        <v>121</v>
+      </c>
+      <c r="C46" t="s" s="34">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="35">
+        <v>123</v>
+      </c>
+      <c r="B47" t="s" s="36">
+        <v>124</v>
+      </c>
+      <c r="C47" t="s" s="37">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="38">
+        <v>126</v>
+      </c>
+      <c r="B48" t="s" s="39">
+        <v>127</v>
+      </c>
+      <c r="C48" t="s" s="40">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s" s="41">
+        <v>79</v>
+      </c>
+      <c r="B49" t="s" s="42">
+        <v>129</v>
+      </c>
+      <c r="C49" t="s" s="43">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s" s="44">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s" s="45">
+        <v>131</v>
+      </c>
+      <c r="C50" t="s" s="46">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s" s="47">
+        <v>133</v>
+      </c>
+      <c r="B51" t="s" s="48">
+        <v>134</v>
+      </c>
+      <c r="C51" t="s" s="49">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s" s="50">
+        <v>136</v>
+      </c>
+      <c r="B52" t="s" s="51">
+        <v>137</v>
+      </c>
+      <c r="C52" t="s" s="52">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s" s="53">
+        <v>138</v>
+      </c>
+      <c r="B53" t="s" s="54">
+        <v>139</v>
+      </c>
+      <c r="C53" t="s" s="55">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s" s="56">
+        <v>56</v>
+      </c>
+      <c r="B54" t="s" s="57">
+        <v>141</v>
+      </c>
+      <c r="C54" t="s" s="58">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s" s="59">
+        <v>56</v>
+      </c>
+      <c r="B55" t="s" s="60">
+        <v>143</v>
+      </c>
+      <c r="C55" t="s" s="61">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s" s="62">
+        <v>136</v>
+      </c>
+      <c r="B56" t="s" s="63">
+        <v>145</v>
+      </c>
+      <c r="C56" t="s" s="64">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s" s="65">
+        <v>136</v>
+      </c>
+      <c r="B57" t="s" s="66">
+        <v>147</v>
+      </c>
+      <c r="C57" t="s" s="67">
+        <v>148</v>
       </c>
     </row>
   </sheetData>

</xml_diff>